<commit_message>
added methods of import from files
</commit_message>
<xml_diff>
--- a/src/test/java/ru/fds/tavrzcms3/testdata/pledge_subject_auto_update.xlsx
+++ b/src/test/java/ru/fds/tavrzcms3/testdata/pledge_subject_auto_update.xlsx
@@ -811,7 +811,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -895,7 +897,7 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>129</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
@@ -957,7 +959,7 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>130</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
@@ -1013,7 +1015,7 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>131</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
         <v>12</v>

</xml_diff>